<commit_message>
mudanças nos cnpj das planilhas
</commit_message>
<xml_diff>
--- a/cypress/fixtures/PlanilhaGTReinf_R-2010testes 1.xlsx
+++ b/cypress/fixtures/PlanilhaGTReinf_R-2010testes 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Mitre\Documents\CypressOpen2.3.2\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\TestesCypress\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09C9DB9-38E7-4C4A-BEB0-7608F29E764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706F2726-C2EB-4B69-8017-05D0FC3909C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GT-Reinf" sheetId="1" r:id="rId1"/>
@@ -107,16 +107,10 @@
     <t>1565922024NP8</t>
   </si>
   <si>
-    <t>03506307000157</t>
-  </si>
-  <si>
     <t>1581222024NP197</t>
   </si>
   <si>
     <t>1552212024NP30</t>
-  </si>
-  <si>
-    <t>04287754000125</t>
   </si>
   <si>
     <t>DDF21</t>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>sim</t>
+  </si>
+  <si>
+    <t>13.574.594/0001-96</t>
+  </si>
+  <si>
+    <t>40.432.544/0001-47</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1003,13 +1003,13 @@
         <v>2708</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="14">
         <v>45779</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="16">
@@ -1018,7 +1018,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="16"/>
       <c r="J3" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3" s="12">
         <v>100000001</v>
@@ -1037,15 +1037,15 @@
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
       <c r="U3" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="V3" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="13">
         <v>1982</v>
@@ -1057,7 +1057,7 @@
         <v>45780</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="16">
@@ -1083,15 +1083,15 @@
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="U4" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="V4" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="12">
         <v>1507</v>
@@ -1103,7 +1103,7 @@
         <v>45781</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="18">
@@ -1128,10 +1128,10 @@
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
       <c r="U5" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="V5" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mudança de teste para produção
</commit_message>
<xml_diff>
--- a/cypress/fixtures/PlanilhaGTReinf_R-2010testes 1.xlsx
+++ b/cypress/fixtures/PlanilhaGTReinf_R-2010testes 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Mitre\Documents\CypressOpen2.3.2\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09C9DB9-38E7-4C4A-BEB0-7608F29E764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD20C5-4478-460D-8BCF-416AA2468F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="14">
-        <v>45779</v>
+        <v>45810</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>23</v>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="14">
-        <v>45780</v>
+        <v>45811</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>23</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="14">
-        <v>45781</v>
+        <v>45812</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>26</v>

</xml_diff>